<commit_message>
Atualizadas Especificações e Adicionados Diagramas da Nadine
</commit_message>
<xml_diff>
--- a/Fase2/UML/Especificação de Use Cases/avaliarServiços.xlsx
+++ b/Fase2/UML/Especificação de Use Cases/avaliarServiços.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Documents\GitHub\li4-17-18\Fase2\UML\Especificação de Use Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8100F579-E46A-42EC-9D95-A76E5B5BAD97}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D60AD5-EDA8-41D6-AD99-29012C35FD28}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{C39B9DE3-7395-4128-8B36-D326E81DB0B8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,26 @@
   </si>
   <si>
     <t>Perfil do pintor atualizado com nova avaliação</t>
+  </si>
+  <si>
+    <t>Excepção 1               (passo 4)
+[Serviço Indisponível]</t>
+  </si>
+  <si>
+    <t>Indica que o serviço pretendido está indisponivel para avaliação</t>
+  </si>
+  <si>
+    <t>Regressa a 3</t>
+  </si>
+  <si>
+    <t>Excepção 2              (passo 6)
+[Avaliação inválida]</t>
+  </si>
+  <si>
+    <t>Regressa a 5</t>
+  </si>
+  <si>
+    <t>Indica que a avaliação é inválida</t>
   </si>
 </sst>
 </file>
@@ -145,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -159,6 +179,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -474,18 +497,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4846AF6-0F24-4F98-854C-62900B086306}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="4" max="4" width="62.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -623,10 +645,68 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6">
+        <v>2</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6">
+        <v>2</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Alteradas Irregualaridades em Diagramas anteriores
</commit_message>
<xml_diff>
--- a/Fase2/UML/Especificação de Use Cases/avaliarServiços.xlsx
+++ b/Fase2/UML/Especificação de Use Cases/avaliarServiços.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Documents\GitHub\li4-17-18\Fase2\UML\Especificação de Use Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D60AD5-EDA8-41D6-AD99-29012C35FD28}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5412953C-4256-4F66-8D53-BE80C05A8B99}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{C39B9DE3-7395-4128-8B36-D326E81DB0B8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -79,26 +79,6 @@
   </si>
   <si>
     <t>Perfil do pintor atualizado com nova avaliação</t>
-  </si>
-  <si>
-    <t>Excepção 1               (passo 4)
-[Serviço Indisponível]</t>
-  </si>
-  <si>
-    <t>Indica que o serviço pretendido está indisponivel para avaliação</t>
-  </si>
-  <si>
-    <t>Regressa a 3</t>
-  </si>
-  <si>
-    <t>Excepção 2              (passo 6)
-[Avaliação inválida]</t>
-  </si>
-  <si>
-    <t>Regressa a 5</t>
-  </si>
-  <si>
-    <t>Indica que a avaliação é inválida</t>
   </si>
 </sst>
 </file>
@@ -500,7 +480,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A15" sqref="A15:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,66 +627,38 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="6">
-        <v>1</v>
-      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="6">
-        <v>2</v>
-      </c>
+      <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="6">
-        <v>1</v>
-      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="6">
-        <v>2</v>
-      </c>
+      <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="D20" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>